<commit_message>
Revert "Merge remote-tracking branch 'origin/田村'"
This reverts commit d428c9bd7479c88758019e33cb522b69d5fa48f2.
</commit_message>
<xml_diff>
--- a/設計書/機能設計/機能設計書.xlsx
+++ b/設計書/機能設計/機能設計書.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81702\Desktop\ntmc\設計書\機能設計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81702\Desktop\資料\Web開発\設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D455E-A3E7-4923-8C85-503EBA5021C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAFCD25-8A46-4929-A6E6-35A80D6A2EEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="3" r:id="rId1"/>
     <sheet name="機能一覧" sheetId="23" r:id="rId2"/>
-    <sheet name="ユーザー画面遷移" sheetId="27" r:id="rId3"/>
-    <sheet name="管理者画面遷移" sheetId="25" r:id="rId4"/>
+    <sheet name="画面推移" sheetId="27" r:id="rId3"/>
+    <sheet name="画面遷移 (2)" sheetId="25" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">機能一覧!$A$1:$H$25</definedName>
@@ -1699,8 +1699,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8131852" y="2204693"/>
-          <a:ext cx="1291634" cy="938584"/>
+          <a:off x="8289499" y="2075709"/>
+          <a:ext cx="1315888" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -1849,8 +1849,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5513007" y="2181214"/>
-          <a:ext cx="1297368" cy="949487"/>
+          <a:off x="5622148" y="2062151"/>
+          <a:ext cx="1321621" cy="889956"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -2059,8 +2059,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8160943" y="4058710"/>
-          <a:ext cx="1291634" cy="949824"/>
+          <a:off x="8318590" y="3820585"/>
+          <a:ext cx="1315888" cy="900215"/>
           <a:chOff x="7154864" y="3068114"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -2265,8 +2265,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4055435" y="5783584"/>
-          <a:ext cx="1291633" cy="946938"/>
+          <a:off x="4128196" y="5446240"/>
+          <a:ext cx="1315886" cy="897329"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -2471,8 +2471,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4089148" y="4012620"/>
-          <a:ext cx="1237498" cy="1082781"/>
+          <a:off x="4161909" y="3784417"/>
+          <a:ext cx="1261751" cy="1013328"/>
           <a:chOff x="2923202" y="1811803"/>
           <a:chExt cx="1523998" cy="910167"/>
         </a:xfrm>
@@ -2717,8 +2717,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8149264" y="6099810"/>
-          <a:ext cx="1287456" cy="941470"/>
+          <a:off x="8306911" y="5742622"/>
+          <a:ext cx="1311710" cy="891861"/>
           <a:chOff x="7788341" y="3625395"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -2915,8 +2915,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10434506" y="2156355"/>
-          <a:ext cx="1237497" cy="1086472"/>
+          <a:off x="10640661" y="2037292"/>
+          <a:ext cx="1261750" cy="1017019"/>
           <a:chOff x="2923202" y="1811803"/>
           <a:chExt cx="1523998" cy="910167"/>
         </a:xfrm>
@@ -3105,8 +3105,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15120938" y="2245650"/>
-          <a:ext cx="1288326" cy="938584"/>
+          <a:off x="15411980" y="2116666"/>
+          <a:ext cx="1324706" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -3247,8 +3247,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4088076" y="7911307"/>
-          <a:ext cx="1291634" cy="948506"/>
+          <a:off x="4160837" y="7454901"/>
+          <a:ext cx="1315887" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -3389,8 +3389,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12555009" y="2232951"/>
-          <a:ext cx="1291632" cy="938584"/>
+          <a:off x="12797543" y="2103967"/>
+          <a:ext cx="1315886" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -3704,8 +3704,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6383602" y="7865270"/>
-          <a:ext cx="1291634" cy="948506"/>
+          <a:off x="6504869" y="7408864"/>
+          <a:ext cx="1315887" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -3822,16 +3822,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>90092</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>143008</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>536576</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>167949</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>79483</xdr:rowOff>
+      <xdr:colOff>9199</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>89404</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3846,8 +3846,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1905795" y="7395899"/>
-          <a:ext cx="1288326" cy="948506"/>
+          <a:off x="1771298" y="7455430"/>
+          <a:ext cx="1324707" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -4076,16 +4076,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>129020</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>579440</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>16194</xdr:rowOff>
+      <xdr:rowOff>18418</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>424029</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>143008</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152930</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4103,8 +4103,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2549958" y="6257053"/>
-          <a:ext cx="1505477" cy="1138846"/>
+          <a:off x="2418750" y="6094711"/>
+          <a:ext cx="1683900" cy="1612529"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4156,8 +4156,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6435990" y="9849115"/>
-          <a:ext cx="1291634" cy="948505"/>
+          <a:off x="6557257" y="9273646"/>
+          <a:ext cx="1315887" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -4298,8 +4298,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4140993" y="9829534"/>
-          <a:ext cx="1291634" cy="938583"/>
+          <a:off x="4213754" y="9254065"/>
+          <a:ext cx="1315887" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -4416,16 +4416,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>79905</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>109670</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>556154</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>40217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>157762</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>36222</xdr:rowOff>
+      <xdr:colOff>28777</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>135441</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4440,8 +4440,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1895608" y="8711936"/>
-          <a:ext cx="1288326" cy="938583"/>
+          <a:off x="1790876" y="9247717"/>
+          <a:ext cx="1324707" cy="888974"/>
           <a:chOff x="5911103" y="2885515"/>
           <a:chExt cx="1295135" cy="945003"/>
         </a:xfrm>
@@ -4558,16 +4558,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>118833</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>79483</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>577158</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>89404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>129020</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>109670</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>596736</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>40217</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4584,9 +4584,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2539771" y="8344405"/>
-          <a:ext cx="10187" cy="367531"/>
+        <a:xfrm>
+          <a:off x="2402783" y="8344404"/>
+          <a:ext cx="19578" cy="903313"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4767,6 +4767,63 @@
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>135441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>596736</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>66146</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="直線コネクタ 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0468746-7C51-4587-B080-3122780805C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="126" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2420938" y="10136691"/>
+          <a:ext cx="1423" cy="406955"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -5072,16 +5129,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>128984</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>372241</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>98536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>361292</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>109140</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5096,8 +5153,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3155156" y="6508067"/>
-          <a:ext cx="837542" cy="853964"/>
+          <a:off x="2824655" y="6339053"/>
+          <a:ext cx="1215258" cy="1248102"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7475,16 +7532,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>232992</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>35923</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>580259</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>356502</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>79716</xdr:rowOff>
+      <xdr:colOff>98534</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>109481</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7499,8 +7556,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2653930" y="8469517"/>
-          <a:ext cx="1333978" cy="549808"/>
+          <a:off x="2419569" y="8933792"/>
+          <a:ext cx="1357586" cy="536465"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7530,7 +7587,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-            <a:t>確認を押下</a:t>
+            <a:t>取り消しを押下</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
         </a:p>
@@ -7598,15 +7655,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>167949</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>111246</xdr:rowOff>
+      <xdr:colOff>9199</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>121167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>59532</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>481724</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
+      <xdr:rowOff>43793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7623,8 +7680,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3194121" y="7870152"/>
-          <a:ext cx="496817" cy="3301879"/>
+          <a:off x="3074716" y="8168150"/>
+          <a:ext cx="472525" cy="2714436"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8015,324 +8072,6 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
             <a:t>ログインを押下</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>58772</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>36222</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>118833</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>158749</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="131" name="直線矢印コネクタ 130">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C24ECED8-3BFF-4C74-9FF3-EDEDFA8E414B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="126" idx="2"/>
-          <a:endCxn id="133" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2479710" y="9650519"/>
-          <a:ext cx="60061" cy="291199"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19844</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>158749</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>97701</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>85301</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="132" name="グループ化 131">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D55F0184-42C1-4ED5-8553-A6AC3831F289}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1835547" y="9941718"/>
-          <a:ext cx="1288326" cy="938583"/>
-          <a:chOff x="5911103" y="2885515"/>
-          <a:chExt cx="1295135" cy="945003"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="133" name="角丸四角形 14">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0218A848-98A0-477E-A046-F750F497F5B6}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5911103" y="2885515"/>
-            <a:ext cx="1295135" cy="945003"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="134" name="テキスト ボックス 133">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E188946B-32EB-4D70-8905-CE7081578F69}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6004485" y="3006912"/>
-            <a:ext cx="1116820" cy="742358"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-              <a:t>【G5-3】</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-              <a:t>予約キャンセル完了画面</a:t>
-            </a:r>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
-          </a:p>
-          <a:p>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
-          </a:p>
-          <a:p>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57381</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>69453</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="135" name="直線コネクタ 134">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{396A2E74-7DB3-400B-81FA-E414E37EE667}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2478319" y="10874375"/>
-          <a:ext cx="12072" cy="297656"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>168671</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>59532</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>292181</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>103324</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="136" name="テキスト ボックス 135">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80BC131-FCA7-4821-8E33-929CA39129F8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2589609" y="9673829"/>
-          <a:ext cx="1333978" cy="549808"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-            <a:t>取り消しを押下</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -15092,8 +14831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7349E5-525C-4988-A10C-1030CDEEAE2C}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="64" workbookViewId="0">
-      <selection activeCell="O68" sqref="O68"/>
+    <sheetView tabSelected="1" zoomScale="36" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>

</xml_diff>